<commit_message>
data updated for wages
</commit_message>
<xml_diff>
--- a/data/source/current_wage.xlsx
+++ b/data/source/current_wage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="570" windowWidth="20775" windowHeight="11955"/>
+    <workbookView xWindow="390" yWindow="570" windowWidth="20775" windowHeight="11955" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Wage Table" sheetId="2" r:id="rId1"/>
@@ -4555,8 +4555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4665,7 +4665,8 @@
         <v>AR</v>
       </c>
       <c r="C7" s="34">
-        <v>669.1</v>
+        <f>+BLS!Q8</f>
+        <v>668.96</v>
       </c>
       <c r="D7" s="33">
         <f>+BLS!T8</f>
@@ -12885,8 +12886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42:D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>